<commit_message>
border fix on timetable
</commit_message>
<xml_diff>
--- a/timetable2.xlsx
+++ b/timetable2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geoal_000\Documents\GitHub\altonbjj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF142B8-ADA7-4AB6-BBF0-DEE98E0C8A3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C38BA8-46C5-46A7-9697-97ECE2636412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4F1D2FA7-6FEE-4329-AE89-E8B36769511D}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -463,6 +463,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -796,7 +799,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:10" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="2"/>
@@ -861,7 +864,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="2"/>

</xml_diff>